<commit_message>
Working Biome weight selection
</commit_message>
<xml_diff>
--- a/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
+++ b/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keeley\git\HexCrawlRepo\HexCrawlGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932DFEB1-6371-405C-B98C-B5DF379D274D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32022920-45F2-4E28-A949-199F598DE5C7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="150">
   <si>
     <t>HexMap - LinkedHashMap&lt;Tuple&lt;Integer&gt;,Hex&gt;</t>
   </si>
@@ -101,9 +101,6 @@
     <t>POTENTIAL FOR: Kingdoms, rulings using biome code modified.</t>
   </si>
   <si>
-    <t>Village</t>
-  </si>
-  <si>
     <t>Generate:</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>Each hex contains:</t>
   </si>
   <si>
-    <t>Territory</t>
-  </si>
-  <si>
     <t>DCs for spotting landmarks, tracks, lairs</t>
   </si>
   <si>
@@ -474,6 +468,15 @@
   </si>
   <si>
     <t>File Reading to input all Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nomad </t>
+  </si>
+  <si>
+    <t>affects all surrounding tiles</t>
+  </si>
+  <si>
+    <t>Town</t>
   </si>
 </sst>
 </file>
@@ -845,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD47954-9054-45D0-8114-DD78AB18C454}">
   <dimension ref="B2:T63"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K26" sqref="K25:K26"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,17 +864,17 @@
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F5" t="s">
         <v>2</v>
@@ -926,15 +929,15 @@
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="Q13" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="Q15" t="s">
+        <v>25</v>
+      </c>
+      <c r="R15" t="s">
         <v>26</v>
-      </c>
-      <c r="R15" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
@@ -945,7 +948,7 @@
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
@@ -958,10 +961,10 @@
         <v>13</v>
       </c>
       <c r="Q18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
@@ -969,39 +972,39 @@
         <v>12</v>
       </c>
       <c r="R19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I23" t="s">
         <v>20</v>
       </c>
       <c r="R23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
@@ -1014,15 +1017,15 @@
         <v>22</v>
       </c>
       <c r="Q25" t="s">
+        <v>38</v>
+      </c>
+      <c r="R25" t="s">
         <v>39</v>
-      </c>
-      <c r="R25" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K26" t="s">
         <v>18</v>
@@ -1033,144 +1036,149 @@
         <v>16</v>
       </c>
       <c r="K27" t="s">
-        <v>24</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K28" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>19</v>
       </c>
-      <c r="K29" t="s">
-        <v>17</v>
-      </c>
       <c r="Q29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="J31" t="s">
-        <v>77</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>147</v>
+      </c>
+      <c r="K32" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
       <c r="Q34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
       <c r="R35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="S36" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="S37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I38" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="S38" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I39" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I42" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="S42" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="S43" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I45" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I46" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I47" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="S47" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="S48" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="3:12" x14ac:dyDescent="0.25">
@@ -1180,74 +1188,74 @@
     </row>
     <row r="51" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K53" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L54" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L55" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L56" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="3:12" x14ac:dyDescent="0.25">
       <c r="L57" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="3:12" x14ac:dyDescent="0.25">
       <c r="L58" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="3:12" x14ac:dyDescent="0.25">
       <c r="L60" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="3:12" x14ac:dyDescent="0.25">
       <c r="L61" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="3:12" x14ac:dyDescent="0.25">
       <c r="L62" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="3:12" x14ac:dyDescent="0.25">
       <c r="L63" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1259,215 +1267,215 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3FFC2E-0279-4607-A621-7B99083CA9F1}">
   <dimension ref="B1:AE45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37:I46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="S6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="S7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.25">
       <c r="S10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="S11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="S12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="T13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="S14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="T16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="AD16" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AE16" s="1"/>
     </row>
     <row r="17" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="U17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AD17" s="1"/>
       <c r="AE17" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="V18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="AD18" s="1"/>
       <c r="AE18" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="2:31" x14ac:dyDescent="0.25">
       <c r="W19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="AD19" s="1"/>
       <c r="AE19" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="S23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="S25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="2:31" x14ac:dyDescent="0.25">
       <c r="T26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="T27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="T28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="2:31" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="T29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="2:31" x14ac:dyDescent="0.25">
       <c r="T30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="T31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="T33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
@@ -1481,58 +1489,58 @@
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F37" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1552,12 +1560,12 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TestBiomeTypes now generates biomes onto the map
</commit_message>
<xml_diff>
--- a/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
+++ b/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keeley\git\HexCrawlRepo\HexCrawlGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32022920-45F2-4E28-A949-199F598DE5C7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DCFC36-3C07-4988-AA58-CC22C0886B35}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="2" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="151">
   <si>
     <t>HexMap - LinkedHashMap&lt;Tuple&lt;Integer&gt;,Hex&gt;</t>
   </si>
@@ -477,6 +477,9 @@
   </si>
   <si>
     <t>Town</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -848,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD47954-9054-45D0-8114-DD78AB18C454}">
   <dimension ref="B2:T63"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25:K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3FFC2E-0279-4607-A621-7B99083CA9F1}">
   <dimension ref="B1:AE45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1550,22 +1553,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFEF3A76-9AB3-444D-84D1-A480A7497687}">
-  <dimension ref="B3:B4"/>
+  <dimension ref="B3:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>145</v>
+      </c>
+      <c r="H4" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring tests into seperate folders
</commit_message>
<xml_diff>
--- a/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
+++ b/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keeley\git\HexCrawlRepo\HexCrawlGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DCFC36-3C07-4988-AA58-CC22C0886B35}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93EDD80A-C23D-41FA-A2EC-4C823AF7F6D1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="2" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="3" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Import File Formats" sheetId="2" r:id="rId2"/>
     <sheet name="Todo" sheetId="6" r:id="rId3"/>
+    <sheet name="BWeights" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="172">
   <si>
     <t>HexMap - LinkedHashMap&lt;Tuple&lt;Integer&gt;,Hex&gt;</t>
   </si>
@@ -480,6 +481,69 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>add random monster lairs to hexes(?)</t>
+  </si>
+  <si>
+    <t>better way to input biome weights, make it non-compulsory to include biomes, make empty indexes = 0</t>
+  </si>
+  <si>
+    <t>TYPE=bweight</t>
+  </si>
+  <si>
+    <t>name=plain</t>
+  </si>
+  <si>
+    <t>scrub</t>
+  </si>
+  <si>
+    <t>forest</t>
+  </si>
+  <si>
+    <t>rough</t>
+  </si>
+  <si>
+    <t>desert</t>
+  </si>
+  <si>
+    <t>hills</t>
+  </si>
+  <si>
+    <t>mountains</t>
+  </si>
+  <si>
+    <t>marsh</t>
+  </si>
+  <si>
+    <t>hell</t>
+  </si>
+  <si>
+    <t>plain=12</t>
+  </si>
+  <si>
+    <t>scrub=3</t>
+  </si>
+  <si>
+    <t>forest=1</t>
+  </si>
+  <si>
+    <t>rough=2</t>
+  </si>
+  <si>
+    <t>desert=3</t>
+  </si>
+  <si>
+    <t>hills=1</t>
+  </si>
+  <si>
+    <t>mountains=1</t>
+  </si>
+  <si>
+    <t>marsh=2</t>
+  </si>
+  <si>
+    <t>hell=0</t>
   </si>
 </sst>
 </file>
@@ -1553,10 +1617,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFEF3A76-9AB3-444D-84D1-A480A7497687}">
-  <dimension ref="B3:H4"/>
+  <dimension ref="B3:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1577,6 +1641,329 @@
         <v>150</v>
       </c>
     </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C3FAB9-666F-4230-B6BA-656A15C724B2}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>7</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>171</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bug fixes, found the abyss generation error.
</commit_message>
<xml_diff>
--- a/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
+++ b/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keeley\git\HexCrawlRepo\HexCrawlGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7899A180-6B00-4289-A542-D456DBA76053}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DA5424-883D-4DED-B60A-3906F8B5E78A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="2" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="4" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Import File Formats" sheetId="2" r:id="rId2"/>
     <sheet name="Todo" sheetId="6" r:id="rId3"/>
     <sheet name="BWeights" sheetId="7" r:id="rId4"/>
+    <sheet name="Classes" sheetId="8" r:id="rId5"/>
+    <sheet name="Generation Order" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="229">
   <si>
     <t>HexMap - LinkedHashMap&lt;Tuple&lt;Integer&gt;,Hex&gt;</t>
   </si>
@@ -489,12 +491,6 @@
     <t>better way to input biome weights, make it non-compulsory to include biomes, make empty indexes = 0</t>
   </si>
   <si>
-    <t>TYPE=bweight</t>
-  </si>
-  <si>
-    <t>name=plain</t>
-  </si>
-  <si>
     <t>scrub</t>
   </si>
   <si>
@@ -519,37 +515,208 @@
     <t>hell</t>
   </si>
   <si>
-    <t>plain=12</t>
-  </si>
-  <si>
-    <t>scrub=3</t>
-  </si>
-  <si>
-    <t>forest=1</t>
-  </si>
-  <si>
-    <t>rough=2</t>
-  </si>
-  <si>
-    <t>desert=3</t>
-  </si>
-  <si>
-    <t>hills=1</t>
-  </si>
-  <si>
-    <t>mountains=1</t>
-  </si>
-  <si>
-    <t>marsh=2</t>
-  </si>
-  <si>
-    <t>hell=0</t>
-  </si>
-  <si>
     <t xml:space="preserve">add River generation </t>
   </si>
   <si>
     <t>draw hex connections n a filled hexmap</t>
+  </si>
+  <si>
+    <t>add decorator pattern to biomes, allow for changes in the biome's stats</t>
+  </si>
+  <si>
+    <t>mountain pass</t>
+  </si>
+  <si>
+    <t>gorge</t>
+  </si>
+  <si>
+    <t>'forested'</t>
+  </si>
+  <si>
+    <t>reefs</t>
+  </si>
+  <si>
+    <t>these are randomly applied to hexes</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>bweight</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>plain</t>
+  </si>
+  <si>
+    <t>Hex has: "WorldObjects" - these affect how the hex is treated by programs.</t>
+  </si>
+  <si>
+    <t>Each has a unique field within the hex.</t>
+  </si>
+  <si>
+    <t>WorldDescriptions - affect the printout of the hex, small additions</t>
+  </si>
+  <si>
+    <t>WorldObject</t>
+  </si>
+  <si>
+    <t>Visibility</t>
+  </si>
+  <si>
+    <t>this affects how far away this object can be seen. If &lt; hex size, only a small chance to see even when within hex.</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>miles wide</t>
+  </si>
+  <si>
+    <t>this affects the encounter table generated by the owning hex, and the neighbouring hexes.</t>
+  </si>
+  <si>
+    <t>visibility is affected by the biome height</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>miles high</t>
+  </si>
+  <si>
+    <t>TravelCost</t>
+  </si>
+  <si>
+    <t>WorldObjects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WorldDescriptors </t>
+  </si>
+  <si>
+    <t>Anything that has affected this hex in some way adds a world descriptor to the hex for outputs.</t>
+  </si>
+  <si>
+    <t>Anything that causes the hex to behave in a unique way to OUTSIDE hexes is a worldobject</t>
+  </si>
+  <si>
+    <t>Affects Hex's base stats, DECORATOR with biome modifier</t>
+  </si>
+  <si>
+    <t>BiomeMod extends Biome</t>
+  </si>
+  <si>
+    <t>Method by which a world object can modify a hex (by decorating it)</t>
+  </si>
+  <si>
+    <t>changes the biomes stats in some way, adding "forested" to name / descriptor etc.</t>
+  </si>
+  <si>
+    <t>Includes:</t>
+  </si>
+  <si>
+    <t>Biomes</t>
+  </si>
+  <si>
+    <t>Initial Biomes are created.</t>
+  </si>
+  <si>
+    <t>Rivers are created, starting from mountains and ending in water hexes</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>WorldDescriptor</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Importance</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>String[]</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Initial Biome modifiers are created to smooth transitions.</t>
+  </si>
+  <si>
+    <t>Smoothers and Transitioners use this to make hybrid biomes</t>
+  </si>
+  <si>
+    <t>Usage:</t>
+  </si>
+  <si>
+    <t>monster,nomadic</t>
+  </si>
+  <si>
+    <t>Ghouls (MM197)</t>
+  </si>
+  <si>
+    <t>Common Monsters present are: Ghouls (MM197), Owlbears and Elephants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This hex is infested(&gt;10 importance) with Rats </t>
+  </si>
+  <si>
+    <t>Nomadic monsters are: Ghouls</t>
+  </si>
+  <si>
+    <t>affects importance of world descriptor</t>
+  </si>
+  <si>
+    <t>-- can't access important stuff like ghoul radius, origin hex etc.</t>
+  </si>
+  <si>
+    <t>Hex Center: 3,1 Radius: 2</t>
+  </si>
+  <si>
+    <t>Monsters - both nomadic and lair-based</t>
+  </si>
+  <si>
+    <t>dungeons - just 1* lair monsters here</t>
+  </si>
+  <si>
+    <t>1..* lair monsters</t>
+  </si>
+  <si>
+    <t>any specified are assumed to regularly leave the dungeon, thus can leave tracks / be fought</t>
+  </si>
+  <si>
+    <t>don't mention all dungeon inhabitants</t>
+  </si>
+  <si>
+    <t>Regions - clump large forests, mountains, water bodies together and have a shared worlddescriptor for those components</t>
+  </si>
+  <si>
+    <t>Roads</t>
+  </si>
+  <si>
+    <t>need to be able to show existing towns connected to this road network</t>
+  </si>
+  <si>
+    <t>each hex MUST be able to get "town directions" via road network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rivers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huge travel cost added </t>
+  </si>
+  <si>
+    <t>Huge pathfinding cost added</t>
   </si>
 </sst>
 </file>
@@ -921,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD47954-9054-45D0-8114-DD78AB18C454}">
   <dimension ref="B2:T63"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25:K28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,6 +1187,9 @@
       <c r="C16" t="s">
         <v>2</v>
       </c>
+      <c r="I16" t="s">
+        <v>173</v>
+      </c>
       <c r="R16" t="s">
         <v>34</v>
       </c>
@@ -1028,10 +1198,16 @@
       <c r="D17" t="s">
         <v>14</v>
       </c>
+      <c r="J17" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>13</v>
+      </c>
+      <c r="J18" t="s">
+        <v>175</v>
       </c>
       <c r="Q18" t="s">
         <v>24</v>
@@ -1623,10 +1799,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFEF3A76-9AB3-444D-84D1-A480A7497687}">
-  <dimension ref="B3:H10"/>
+  <dimension ref="B3:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1659,12 +1835,42 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>173</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1674,10 +1880,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C3FAB9-666F-4230-B6BA-656A15C724B2}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1685,46 +1891,52 @@
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D2" t="s">
         <v>154</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>155</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>156</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>157</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>158</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>159</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>160</v>
       </c>
-      <c r="H2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1745,22 +1957,25 @@
         <v>1</v>
       </c>
       <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
         <v>8</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>2</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
       <c r="E4">
         <v>1</v>
       </c>
@@ -1774,28 +1989,31 @@
         <v>1</v>
       </c>
       <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>10</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
       <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>0</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
       <c r="G5">
         <v>1</v>
       </c>
@@ -1803,73 +2021,82 @@
         <v>1</v>
       </c>
       <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>3</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>2</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>4</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>2</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
       <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
         <v>2</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>3</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>6</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
       <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>2</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
       <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1878,24 +2105,27 @@
         <v>2</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
         <v>6</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>2</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
       <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1904,27 +2134,30 @@
         <v>1</v>
       </c>
       <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <v>2</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
       <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
         <v>4</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>8</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1933,27 +2166,30 @@
         <v>2</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
         <v>0</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
       <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
         <v>0</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>7</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1965,10 +2201,10 @@
         <v>0</v>
       </c>
       <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>10</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1977,7 +2213,281 @@
         <v>0</v>
       </c>
       <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7658268-425E-4714-A5A5-378B4A74F2DC}">
+  <dimension ref="B2:W34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>190</v>
+      </c>
+      <c r="W3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E4" t="s">
+        <v>184</v>
+      </c>
+      <c r="J4" t="s">
+        <v>186</v>
+      </c>
+      <c r="L4" t="s">
+        <v>189</v>
+      </c>
+      <c r="W4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>185</v>
+      </c>
+      <c r="J5" t="s">
+        <v>187</v>
+      </c>
+      <c r="L5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>194</v>
+      </c>
+      <c r="W6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="N7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>177</v>
+      </c>
+      <c r="E14" t="s">
+        <v>178</v>
+      </c>
+      <c r="R14" t="s">
+        <v>223</v>
+      </c>
+      <c r="S14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>181</v>
+      </c>
+      <c r="S15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>214</v>
+      </c>
+      <c r="R17" t="s">
+        <v>226</v>
+      </c>
+      <c r="S17" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="S18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="S23" t="s">
+        <v>219</v>
+      </c>
+      <c r="U23" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U24" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>205</v>
+      </c>
+      <c r="D26" t="s">
+        <v>198</v>
+      </c>
+      <c r="G26" t="s">
+        <v>208</v>
+      </c>
+      <c r="H26" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>203</v>
+      </c>
+      <c r="D27" t="s">
+        <v>202</v>
+      </c>
+      <c r="H27" t="s">
+        <v>209</v>
+      </c>
+      <c r="R27" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>205</v>
+      </c>
+      <c r="D28" t="s">
+        <v>200</v>
+      </c>
+      <c r="H28" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>204</v>
+      </c>
+      <c r="D29" t="s">
+        <v>201</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K31" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="34" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533EBB87-5A6A-46A2-9F13-A4D39854AC7D}">
+  <dimension ref="C4:M6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>206</v>
+      </c>
+      <c r="L5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>197</v>
+      </c>
+      <c r="M6" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Setting up hex storages and road networks
</commit_message>
<xml_diff>
--- a/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
+++ b/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keeley\git\HexCrawlRepo\HexCrawlGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DA5424-883D-4DED-B60A-3906F8B5E78A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13495825-F64E-4EE0-A6F1-58BBCC60DC57}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="4" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="230">
   <si>
     <t>HexMap - LinkedHashMap&lt;Tuple&lt;Integer&gt;,Hex&gt;</t>
   </si>
@@ -713,10 +713,13 @@
     <t xml:space="preserve">Rivers </t>
   </si>
   <si>
-    <t xml:space="preserve">Huge travel cost added </t>
-  </si>
-  <si>
     <t>Huge pathfinding cost added</t>
+  </si>
+  <si>
+    <t>input current hex, get towns and the direction along what road</t>
+  </si>
+  <si>
+    <t>Huge travel cost added (bridge ignores this)</t>
   </si>
 </sst>
 </file>
@@ -2229,7 +2232,7 @@
   <dimension ref="B2:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,26 +2342,29 @@
       <c r="E16" t="s">
         <v>182</v>
       </c>
+      <c r="S16" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>214</v>
       </c>
-      <c r="R17" t="s">
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R18" t="s">
         <v>226</v>
       </c>
-      <c r="S17" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="S18" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>199</v>
+      </c>
+      <c r="S19" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revert "Setting up hex storages and road networks"
This reverts commit 734ae835e339ae6327e31f119b68d580723b96cf.
</commit_message>
<xml_diff>
--- a/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
+++ b/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keeley\git\HexCrawlRepo\HexCrawlGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13495825-F64E-4EE0-A6F1-58BBCC60DC57}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DA5424-883D-4DED-B60A-3906F8B5E78A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="4" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="229">
   <si>
     <t>HexMap - LinkedHashMap&lt;Tuple&lt;Integer&gt;,Hex&gt;</t>
   </si>
@@ -713,13 +713,10 @@
     <t xml:space="preserve">Rivers </t>
   </si>
   <si>
+    <t xml:space="preserve">Huge travel cost added </t>
+  </si>
+  <si>
     <t>Huge pathfinding cost added</t>
-  </si>
-  <si>
-    <t>input current hex, get towns and the direction along what road</t>
-  </si>
-  <si>
-    <t>Huge travel cost added (bridge ignores this)</t>
   </si>
 </sst>
 </file>
@@ -2232,7 +2229,7 @@
   <dimension ref="B2:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2342,29 +2339,26 @@
       <c r="E16" t="s">
         <v>182</v>
       </c>
-      <c r="S16" t="s">
-        <v>228</v>
-      </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>214</v>
       </c>
+      <c r="R17" t="s">
+        <v>226</v>
+      </c>
+      <c r="S17" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R18" t="s">
-        <v>226</v>
-      </c>
       <c r="S18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>199</v>
-      </c>
-      <c r="S19" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Large refactoring of code, descriptors and properties
</commit_message>
<xml_diff>
--- a/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
+++ b/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keeley\git\HexCrawlRepo\HexCrawlGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13495825-F64E-4EE0-A6F1-58BBCC60DC57}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4C7A8A-E3DC-4747-9B9A-7E1B3391AE23}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="4" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="238">
   <si>
     <t>HexMap - LinkedHashMap&lt;Tuple&lt;Integer&gt;,Hex&gt;</t>
   </si>
@@ -720,6 +720,30 @@
   </si>
   <si>
     <t>Huge travel cost added (bridge ignores this)</t>
+  </si>
+  <si>
+    <t>Roads:</t>
+  </si>
+  <si>
+    <t>towns and similar generate "RoadNodes" at their Point</t>
+  </si>
+  <si>
+    <t>Connection controller then joins up all roadnodes within travel distance of one another</t>
+  </si>
+  <si>
+    <t>Creates roadnetworks of these sets</t>
+  </si>
+  <si>
+    <t>Find towns along these roads</t>
+  </si>
+  <si>
+    <t>RoadNode used to tell other hexes that it has a road.</t>
+  </si>
+  <si>
+    <t>ValidStart</t>
+  </si>
+  <si>
+    <t>If head can start with this biome (not good for rare biomes)</t>
   </si>
 </sst>
 </file>
@@ -2232,7 +2256,7 @@
   <dimension ref="B2:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2250,10 +2274,7 @@
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E3" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="J3" t="s">
         <v>3</v>
@@ -2267,10 +2288,7 @@
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>183</v>
-      </c>
-      <c r="E4" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="J4" t="s">
         <v>186</v>
@@ -2284,7 +2302,10 @@
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>185</v>
+        <v>179</v>
+      </c>
+      <c r="E5" t="s">
+        <v>180</v>
       </c>
       <c r="J5" t="s">
         <v>187</v>
@@ -2294,6 +2315,12 @@
       </c>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E6" t="s">
+        <v>184</v>
+      </c>
       <c r="M6" t="s">
         <v>194</v>
       </c>
@@ -2302,11 +2329,20 @@
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>185</v>
+      </c>
       <c r="N7" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>236</v>
+      </c>
+      <c r="E8" t="s">
+        <v>237</v>
+      </c>
       <c r="N8" t="s">
         <v>186</v>
       </c>
@@ -2349,6 +2385,9 @@
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>214</v>
+      </c>
+      <c r="S17" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
@@ -2467,20 +2506,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533EBB87-5A6A-46A2-9F13-A4D39854AC7D}">
-  <dimension ref="C4:M6"/>
+  <dimension ref="C4:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="P16" sqref="L12:P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>206</v>
       </c>
@@ -2488,12 +2527,37 @@
         <v>217</v>
       </c>
     </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>197</v>
       </c>
       <c r="M6" t="s">
         <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More refactoring and inheritance for worldobjects.
</commit_message>
<xml_diff>
--- a/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
+++ b/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keeley\git\HexCrawlRepo\HexCrawlGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4C7A8A-E3DC-4747-9B9A-7E1B3391AE23}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58403D5-5244-4355-95C4-4832383E5E6A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="4" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="8" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,10 @@
     <sheet name="Todo" sheetId="6" r:id="rId3"/>
     <sheet name="BWeights" sheetId="7" r:id="rId4"/>
     <sheet name="Classes" sheetId="8" r:id="rId5"/>
-    <sheet name="Generation Order" sheetId="9" r:id="rId6"/>
+    <sheet name="TodoList" sheetId="10" r:id="rId6"/>
+    <sheet name="Properties" sheetId="11" r:id="rId7"/>
+    <sheet name="Generation Order" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet3" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="367">
   <si>
     <t>HexMap - LinkedHashMap&lt;Tuple&lt;Integer&gt;,Hex&gt;</t>
   </si>
@@ -744,6 +747,393 @@
   </si>
   <si>
     <t>If head can start with this biome (not good for rare biomes)</t>
+  </si>
+  <si>
+    <t>Features to Code</t>
+  </si>
+  <si>
+    <t>Features finished</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add "do not start" biomes </t>
+  </si>
+  <si>
+    <t>Generation:</t>
+  </si>
+  <si>
+    <t>Editing:</t>
+  </si>
+  <si>
+    <t>Save/Load hexmap with serialization</t>
+  </si>
+  <si>
+    <t>Outputting:</t>
+  </si>
+  <si>
+    <t>Add River Generation</t>
+  </si>
+  <si>
+    <t>Add Road Generation</t>
+  </si>
+  <si>
+    <t>Add Monster Generation</t>
+  </si>
+  <si>
+    <t>Monster:</t>
+  </si>
+  <si>
+    <t>NomadChance:</t>
+  </si>
+  <si>
+    <t>Description:</t>
+  </si>
+  <si>
+    <t>RoamingRadius:</t>
+  </si>
+  <si>
+    <t>applies to both nomadic and lairs</t>
+  </si>
+  <si>
+    <t>SpawnChance: &lt;biomename&gt;-X</t>
+  </si>
+  <si>
+    <t>SpawnChance: &lt;biomename&gt;-X, &lt;b2&gt;-X</t>
+  </si>
+  <si>
+    <t>Visibility:</t>
+  </si>
+  <si>
+    <t>Valid Starts:</t>
+  </si>
+  <si>
+    <t>Elevated Water sources</t>
+  </si>
+  <si>
+    <t>Mountains</t>
+  </si>
+  <si>
+    <t>Valid Ends:</t>
+  </si>
+  <si>
+    <t>Low water sources</t>
+  </si>
+  <si>
+    <t>Features:</t>
+  </si>
+  <si>
+    <t>"Generates random maps with custom biomes"</t>
+  </si>
+  <si>
+    <t>"Biomes will influence others nearby, sharing properties and transitioning smoothly"</t>
+  </si>
+  <si>
+    <t>"Adds terrain features such as towns, dungeons, lairs, roaming monsters, roads and rivers"</t>
+  </si>
+  <si>
+    <t>"Creates a auto-generated d100 encounter list for each hex"</t>
+  </si>
+  <si>
+    <t>"Gives information of surrounding hexes based on what the players could see"</t>
+  </si>
+  <si>
+    <t>"Create custom encounter lists for worldobjects that the generator will insert"</t>
+  </si>
+  <si>
+    <t>Add Custom Encounters to replace standard encounters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encounters </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0..* </t>
+  </si>
+  <si>
+    <t>uses this list when adding encounters to the d100 list, replaces standard "there are ghouls here"</t>
+  </si>
+  <si>
+    <t>FUNCTIONALITY</t>
+  </si>
+  <si>
+    <t>Rivers</t>
+  </si>
+  <si>
+    <t>Link different hexes together</t>
+  </si>
+  <si>
+    <t>Link towns together</t>
+  </si>
+  <si>
+    <t>Generate signposts for directions</t>
+  </si>
+  <si>
+    <t>Act as boundaries to monsters</t>
+  </si>
+  <si>
+    <t>Increase travel cost</t>
+  </si>
+  <si>
+    <t>Generate crossings on rivers (remove travel cost)</t>
+  </si>
+  <si>
+    <t>Add biome modificators from file</t>
+  </si>
+  <si>
+    <t>Add biome modificators from worldobjects</t>
+  </si>
+  <si>
+    <t>Add River and Road nodes</t>
+  </si>
+  <si>
+    <t>Add town and landmark Gen</t>
+  </si>
+  <si>
+    <t>cannot 'swim' down rivers, as they are not biomes.</t>
+  </si>
+  <si>
+    <t>Travelcost affects 'land' creatures</t>
+  </si>
+  <si>
+    <t>Fly or Other</t>
+  </si>
+  <si>
+    <t>RoamType:</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>travelcost</t>
+  </si>
+  <si>
+    <t>spotdistance</t>
+  </si>
+  <si>
+    <t>riverorigin</t>
+  </si>
+  <si>
+    <t>riverend</t>
+  </si>
+  <si>
+    <t>Lair or nomadic</t>
+  </si>
+  <si>
+    <t>Chance is RandInt(1,100), if result &lt; chance, thing happens.</t>
+  </si>
+  <si>
+    <t>X% chance PER hex of that biome type.</t>
+  </si>
+  <si>
+    <t>BiomeModifier:</t>
+  </si>
+  <si>
+    <t>ADDS to modified biome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Color: </t>
+  </si>
+  <si>
+    <t>adds this component to each</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name: </t>
+  </si>
+  <si>
+    <t>(Prefix)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">height: </t>
+  </si>
+  <si>
+    <t>adds if positive, takes if negative</t>
+  </si>
+  <si>
+    <t>as above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spotdistance </t>
+  </si>
+  <si>
+    <t>encounters will be encountered at this distance within the hex (ft)</t>
+  </si>
+  <si>
+    <t>aka, stealth rolls should be rolled at this distance, failure = this distance spotted.</t>
+  </si>
+  <si>
+    <t>spot should be a diceroll string</t>
+  </si>
+  <si>
+    <t>flat integer</t>
+  </si>
+  <si>
+    <t>validbiomes:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">origin: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">will only apply this biome to valid biomes </t>
+  </si>
+  <si>
+    <t>searches via name, regardless of type.</t>
+  </si>
+  <si>
+    <t>Biomes only</t>
+  </si>
+  <si>
+    <t>biome names csv</t>
+  </si>
+  <si>
+    <t>&lt;biomename&gt;-X</t>
+  </si>
+  <si>
+    <t>Affected by travel cost, does a "flood" search to find radius</t>
+  </si>
+  <si>
+    <t>Town:</t>
+  </si>
+  <si>
+    <t>(Lair)</t>
+  </si>
+  <si>
+    <t>no lairs, create 0 nomadicchance monsters to always generate a lair.</t>
+  </si>
+  <si>
+    <t>if additional flavor required, use dungeons instead.</t>
+  </si>
+  <si>
+    <t>Landmark</t>
+  </si>
+  <si>
+    <t>PRE-SET MODIFIERS THAT OCCUR WITHIN PROGRAM</t>
+  </si>
+  <si>
+    <t>Adds, use 1 sentence./</t>
+  </si>
+  <si>
+    <t>Use full sentences, 3 maximum probably.</t>
+  </si>
+  <si>
+    <t>SpawnChance:</t>
+  </si>
+  <si>
+    <t>lair monsters that can be present</t>
+  </si>
+  <si>
+    <t>how dominant evidence of these tracks are</t>
+  </si>
+  <si>
+    <t>Likelihood of encountering tracks or evidence, not the monster itself.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MonsterChance: </t>
+  </si>
+  <si>
+    <t>&lt;monstername&gt;-X, &lt;monstername&gt;-X</t>
+  </si>
+  <si>
+    <t>affects river generation</t>
+  </si>
+  <si>
+    <t>Some minor modifiers such as river origins only add description, not name.</t>
+  </si>
+  <si>
+    <t>Connectivity:</t>
+  </si>
+  <si>
+    <t>The resource it uses to create a road to nearby town(s)</t>
+  </si>
+  <si>
+    <t>Visibility affects how well it is seen within and nearby its home hex. Large visibility means it'll appear on more encounter tables as "evidence"</t>
+  </si>
+  <si>
+    <t>EncounterChance:</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>EVIDENCE</t>
+  </si>
+  <si>
+    <t>appends any monsters as 'patrols'</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>MinMax</t>
+  </si>
+  <si>
+    <t>&lt;Min,Max&gt;</t>
+  </si>
+  <si>
+    <t>After generation, finds clusters of valid biomes and labels them with a region</t>
+  </si>
+  <si>
+    <t>This is mainly for lore</t>
+  </si>
+  <si>
+    <t>MinSize</t>
+  </si>
+  <si>
+    <t>How many hexes of validbiomes together before this is considered a valid region location.</t>
+  </si>
+  <si>
+    <t>InitialPath=true</t>
+  </si>
+  <si>
+    <t>If can reach nearest town</t>
+  </si>
+  <si>
+    <t>While initialpath=false</t>
+  </si>
+  <si>
+    <t>Get next largest connectivity</t>
+  </si>
+  <si>
+    <t>update townQ</t>
+  </si>
+  <si>
+    <t>While contains towns in townQ</t>
+  </si>
+  <si>
+    <t>If can reach nearest town or roadnode</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>remove town from townQ</t>
+  </si>
+  <si>
+    <t>subtract connectivity from BOTH</t>
+  </si>
+  <si>
+    <t>(do not subtract connectivity for initial path)</t>
+  </si>
+  <si>
+    <t>Sort Towns by largest connectivity TownQ</t>
+  </si>
+  <si>
+    <t>Get largest Town (or next largest)</t>
+  </si>
+  <si>
+    <t>Road Generator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROADPath to nearest town </t>
+  </si>
+  <si>
+    <t>ROADconnect to nearest town OR roadnode</t>
+  </si>
+  <si>
+    <t>Dijkstra's</t>
+  </si>
+  <si>
+    <t>search through connections for hexes containing towns, if they do</t>
   </si>
 </sst>
 </file>
@@ -1544,7 +1934,7 @@
   <dimension ref="B1:AE45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:G17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2255,8 +2645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7658268-425E-4714-A5A5-378B4A74F2DC}">
   <dimension ref="B2:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2406,6 +2796,17 @@
         <v>227</v>
       </c>
     </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>269</v>
+      </c>
+      <c r="E20" t="s">
+        <v>270</v>
+      </c>
+      <c r="F20" t="s">
+        <v>271</v>
+      </c>
+    </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="R22" t="s">
         <v>22</v>
@@ -2505,11 +2906,548 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66146DA2-A49A-4A2A-BD60-539D5A363125}">
+  <dimension ref="A1:Q22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E1" t="s">
+        <v>239</v>
+      </c>
+      <c r="N1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>241</v>
+      </c>
+      <c r="O3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>240</v>
+      </c>
+      <c r="N4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>245</v>
+      </c>
+      <c r="O5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>283</v>
+      </c>
+      <c r="N6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>246</v>
+      </c>
+      <c r="O7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>268</v>
+      </c>
+      <c r="N12" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N13" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N14" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>242</v>
+      </c>
+      <c r="N15" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>243</v>
+      </c>
+      <c r="N16" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E41E48A-940E-466C-A207-70F5A6CF197C}">
+  <dimension ref="B1:W43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T43" sqref="T43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>295</v>
+      </c>
+      <c r="N1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>340</v>
+      </c>
+      <c r="R2" t="s">
+        <v>320</v>
+      </c>
+      <c r="S2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>248</v>
+      </c>
+      <c r="P4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Q6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E9" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>335</v>
+      </c>
+      <c r="S9" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>251</v>
+      </c>
+      <c r="E10" t="s">
+        <v>252</v>
+      </c>
+      <c r="I10" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>254</v>
+      </c>
+      <c r="H11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>255</v>
+      </c>
+      <c r="D12" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>287</v>
+      </c>
+      <c r="D13" t="s">
+        <v>286</v>
+      </c>
+      <c r="F13" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>338</v>
+      </c>
+      <c r="E15" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="P17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>200</v>
+      </c>
+      <c r="E19" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>200</v>
+      </c>
+      <c r="S19" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>327</v>
+      </c>
+      <c r="S20" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>331</v>
+      </c>
+      <c r="S21" t="s">
+        <v>332</v>
+      </c>
+      <c r="W21" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>177</v>
+      </c>
+      <c r="W22" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>291</v>
+      </c>
+      <c r="E23" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>292</v>
+      </c>
+      <c r="F24" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>293</v>
+      </c>
+      <c r="F25" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>297</v>
+      </c>
+      <c r="D28" t="s">
+        <v>298</v>
+      </c>
+      <c r="P28" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>301</v>
+      </c>
+      <c r="D29" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>250</v>
+      </c>
+      <c r="D30" t="s">
+        <v>325</v>
+      </c>
+      <c r="G30" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>299</v>
+      </c>
+      <c r="D31" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>303</v>
+      </c>
+      <c r="D32" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>290</v>
+      </c>
+      <c r="D33" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="34" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>306</v>
+      </c>
+      <c r="D34" t="s">
+        <v>305</v>
+      </c>
+      <c r="G34" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="35" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>311</v>
+      </c>
+      <c r="G35" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="36" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>312</v>
+      </c>
+      <c r="D36" t="s">
+        <v>317</v>
+      </c>
+      <c r="F36" t="s">
+        <v>316</v>
+      </c>
+      <c r="H36" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="37" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>292</v>
+      </c>
+      <c r="E37" t="s">
+        <v>333</v>
+      </c>
+      <c r="I37" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="38" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>293</v>
+      </c>
+      <c r="E38" t="s">
+        <v>333</v>
+      </c>
+      <c r="I38" t="s">
+        <v>324</v>
+      </c>
+      <c r="P38" t="s">
+        <v>342</v>
+      </c>
+      <c r="T38" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="39" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="Q39" t="s">
+        <v>198</v>
+      </c>
+      <c r="U39" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="40" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="Q40" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="Q41" t="s">
+        <v>343</v>
+      </c>
+      <c r="R41" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="42" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="Q42" t="s">
+        <v>347</v>
+      </c>
+      <c r="R42" t="s">
+        <v>339</v>
+      </c>
+      <c r="T42" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="43" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="Q43" t="s">
+        <v>311</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533EBB87-5A6A-46A2-9F13-A4D39854AC7D}">
   <dimension ref="C4:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P16" sqref="L12:P16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2535,7 +3473,30 @@
         <v>218</v>
       </c>
     </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>259</v>
+      </c>
+    </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>260</v>
+      </c>
       <c r="L12" t="s">
         <v>230</v>
       </c>
@@ -2558,6 +3519,110 @@
     <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="N16" t="s">
         <v>234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD20796D-B0DE-4732-BD5F-0F3C623F8AF6}">
+  <dimension ref="B1:I17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>350</v>
+      </c>
+      <c r="H5" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>355</v>
+      </c>
+      <c r="H12" t="s">
+        <v>365</v>
+      </c>
+      <c r="I12" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds biome chooser class instead of bweights
</commit_message>
<xml_diff>
--- a/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
+++ b/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keeley\git\HexCrawlRepo\HexCrawlGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB3A742-1C62-47D1-8CED-C8676E9A99E8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23056732-8B14-4F22-8E74-30BF61B562B1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="6" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
   </bookViews>
@@ -3538,7 +3538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E41E48A-940E-466C-A207-70F5A6CF197C}">
   <dimension ref="B1:W43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Some base monster implementation,
fleshes out how monsters will be stored
</commit_message>
<xml_diff>
--- a/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
+++ b/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keeley\git\HexCrawlRepo\HexCrawlGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23056732-8B14-4F22-8E74-30BF61B562B1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1FF2D8-D1F4-4638-A6CB-064004DF596C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="6" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
   </bookViews>
@@ -22,7 +22,6 @@
     <sheet name="Properties" sheetId="11" r:id="rId7"/>
     <sheet name="Generation Order" sheetId="9" r:id="rId8"/>
     <sheet name="Sheet3" sheetId="12" r:id="rId9"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="386">
   <si>
     <t>HexMap - LinkedHashMap&lt;Tuple&lt;Integer&gt;,Hex&gt;</t>
   </si>
@@ -1137,13 +1136,61 @@
     <t>search through connections for hexes containing towns, if they do</t>
   </si>
   <si>
-    <t>abyss</t>
-  </si>
-  <si>
-    <t>water</t>
-  </si>
-  <si>
-    <t>reef</t>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>&lt;biomename&gt;-X,&lt;biomename2&gt;-X2</t>
+  </si>
+  <si>
+    <t>Add biome modifications from File</t>
+  </si>
+  <si>
+    <t>Add Custom Encounters to replace standard "encounter a monster"</t>
+  </si>
+  <si>
+    <t>Add initial biome modifiers</t>
+  </si>
+  <si>
+    <t>generate rivers</t>
+  </si>
+  <si>
+    <t>generate biomes</t>
+  </si>
+  <si>
+    <t>generate towns and landmarks</t>
+  </si>
+  <si>
+    <t>generate roads</t>
+  </si>
+  <si>
+    <t>Add monsters to hexes</t>
+  </si>
+  <si>
+    <t>Add river biome modifiers to biomes</t>
+  </si>
+  <si>
+    <t>HexRoller</t>
+  </si>
+  <si>
+    <t>HashMap&lt;Biome,</t>
+  </si>
+  <si>
+    <t>Don’t need rivers and roads to be rolled, hexes handle that themselves.</t>
+  </si>
+  <si>
+    <t>if this is successfully rolled for the hex, apply that biomemod to all adjacent valid hexes</t>
+  </si>
+  <si>
+    <t>RandomCollection&lt;BiomeMods&gt;&gt; mods</t>
+  </si>
+  <si>
+    <t>RandomCollection&lt;Monster&gt;&gt; monsters</t>
+  </si>
+  <si>
+    <t>if this is successfully rolled for the hex, add that monster to this hex</t>
+  </si>
+  <si>
+    <t>RandomCollection&lt;Biome&gt;&gt; biomes</t>
   </si>
 </sst>
 </file>
@@ -1194,14 +1241,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1942,480 +1986,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB24C8B8-13DD-4866-A847-9EE60EC0784A}">
-  <dimension ref="A1:L12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="A1:L12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="12" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>367</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="B2" s="4">
-        <v>500</v>
-      </c>
-      <c r="C2" s="4">
-        <v>10</v>
-      </c>
-      <c r="D2" s="4">
-        <v>10</v>
-      </c>
-      <c r="E2" s="4">
-        <v>1</v>
-      </c>
-      <c r="F2" s="4">
-        <v>1</v>
-      </c>
-      <c r="G2" s="4">
-        <v>1</v>
-      </c>
-      <c r="H2" s="4">
-        <v>1</v>
-      </c>
-      <c r="I2" s="4">
-        <v>1</v>
-      </c>
-      <c r="J2" s="4">
-        <v>0</v>
-      </c>
-      <c r="K2" s="4">
-        <v>1</v>
-      </c>
-      <c r="L2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="B3" s="4">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4">
-        <v>500</v>
-      </c>
-      <c r="D3" s="4">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4">
-        <v>1</v>
-      </c>
-      <c r="H3" s="4">
-        <v>1</v>
-      </c>
-      <c r="I3" s="4">
-        <v>1</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0</v>
-      </c>
-      <c r="K3" s="4">
-        <v>1</v>
-      </c>
-      <c r="L3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B4" s="4">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4">
-        <v>500</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="4">
-        <v>1</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0</v>
-      </c>
-      <c r="K4" s="4">
-        <v>1</v>
-      </c>
-      <c r="L4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4">
-        <v>50</v>
-      </c>
-      <c r="F5" s="4">
-        <v>5</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1</v>
-      </c>
-      <c r="I5" s="4">
-        <v>0</v>
-      </c>
-      <c r="J5" s="4">
-        <v>1</v>
-      </c>
-      <c r="K5" s="4">
-        <v>1</v>
-      </c>
-      <c r="L5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>5</v>
-      </c>
-      <c r="F6" s="4">
-        <v>100</v>
-      </c>
-      <c r="G6" s="4">
-        <v>1</v>
-      </c>
-      <c r="H6" s="4">
-        <v>1</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0</v>
-      </c>
-      <c r="J6" s="4">
-        <v>1</v>
-      </c>
-      <c r="K6" s="4">
-        <v>1</v>
-      </c>
-      <c r="L6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="B7" s="4">
-        <v>100</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4">
-        <v>100</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1</v>
-      </c>
-      <c r="F7" s="4">
-        <v>10</v>
-      </c>
-      <c r="G7" s="4">
-        <v>500</v>
-      </c>
-      <c r="H7" s="4">
-        <v>1</v>
-      </c>
-      <c r="I7" s="4">
-        <v>1</v>
-      </c>
-      <c r="J7" s="4">
-        <v>0</v>
-      </c>
-      <c r="K7" s="4">
-        <v>1</v>
-      </c>
-      <c r="L7" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4">
-        <v>5</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4">
-        <v>1</v>
-      </c>
-      <c r="H8" s="4">
-        <v>500</v>
-      </c>
-      <c r="I8" s="4">
-        <v>1</v>
-      </c>
-      <c r="J8" s="4">
-        <v>0</v>
-      </c>
-      <c r="K8" s="4">
-        <v>1</v>
-      </c>
-      <c r="L8" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B9" s="4">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>10</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
-        <v>50</v>
-      </c>
-      <c r="J9" s="4">
-        <v>0</v>
-      </c>
-      <c r="K9" s="4">
-        <v>1</v>
-      </c>
-      <c r="L9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>367</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>5</v>
-      </c>
-      <c r="F10" s="4">
-        <v>5</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0</v>
-      </c>
-      <c r="I10" s="4">
-        <v>0</v>
-      </c>
-      <c r="J10" s="4">
-        <v>1</v>
-      </c>
-      <c r="K10" s="4">
-        <v>0</v>
-      </c>
-      <c r="L10" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="B11" s="4">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1</v>
-      </c>
-      <c r="E11" s="4">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1</v>
-      </c>
-      <c r="G11" s="4">
-        <v>1</v>
-      </c>
-      <c r="H11" s="4">
-        <v>1</v>
-      </c>
-      <c r="I11" s="4">
-        <v>1</v>
-      </c>
-      <c r="J11" s="4">
-        <v>0</v>
-      </c>
-      <c r="K11" s="4">
-        <v>300</v>
-      </c>
-      <c r="L11" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="B12" s="4">
-        <v>0</v>
-      </c>
-      <c r="C12" s="4">
-        <v>0</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4">
-        <v>0</v>
-      </c>
-      <c r="G12" s="4">
-        <v>0</v>
-      </c>
-      <c r="H12" s="4">
-        <v>0</v>
-      </c>
-      <c r="I12" s="4">
-        <v>0</v>
-      </c>
-      <c r="J12" s="4">
-        <v>0</v>
-      </c>
-      <c r="K12" s="4">
-        <v>10</v>
-      </c>
-      <c r="L12" s="4">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3FFC2E-0279-4607-A621-7B99083CA9F1}">
   <dimension ref="B1:AE45"/>
@@ -3130,10 +2700,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7658268-425E-4714-A5A5-378B4A74F2DC}">
-  <dimension ref="B2:W34"/>
+  <dimension ref="B2:W45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3377,14 +2947,59 @@
         <v>212</v>
       </c>
     </row>
-    <row r="33" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J33" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J34" t="s">
         <v>213</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>379</v>
+      </c>
+      <c r="E42" t="s">
+        <v>383</v>
+      </c>
+      <c r="J42" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>379</v>
+      </c>
+      <c r="E43" t="s">
+        <v>382</v>
+      </c>
+      <c r="J43" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>379</v>
+      </c>
+      <c r="E44" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -3397,7 +3012,7 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A4" sqref="A4:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3538,8 +3153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E41E48A-940E-466C-A207-70F5A6CF197C}">
   <dimension ref="B1:W43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3760,6 +3375,14 @@
         <v>309</v>
       </c>
     </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>367</v>
+      </c>
+      <c r="D26" t="s">
+        <v>368</v>
+      </c>
+    </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>297</v>
@@ -3931,10 +3554,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533EBB87-5A6A-46A2-9F13-A4D39854AC7D}">
-  <dimension ref="C4:N16"/>
+  <dimension ref="C4:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4006,6 +3629,51 @@
     <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="N16" t="s">
         <v>234</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rivers now generate, many, many problems still present.
</commit_message>
<xml_diff>
--- a/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
+++ b/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keeley\git\HexCrawlRepo\HexCrawlGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1FF2D8-D1F4-4638-A6CB-064004DF596C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C233FC8-A551-4DBE-999E-05FAC17F35BD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="6" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="3" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Import File Formats" sheetId="2" r:id="rId2"/>
     <sheet name="Todo" sheetId="6" r:id="rId3"/>
-    <sheet name="BWeights" sheetId="7" r:id="rId4"/>
-    <sheet name="Classes" sheetId="8" r:id="rId5"/>
-    <sheet name="TodoList" sheetId="10" r:id="rId6"/>
-    <sheet name="Properties" sheetId="11" r:id="rId7"/>
-    <sheet name="Generation Order" sheetId="9" r:id="rId8"/>
-    <sheet name="Sheet3" sheetId="12" r:id="rId9"/>
+    <sheet name="Classes" sheetId="8" r:id="rId4"/>
+    <sheet name="TodoList" sheetId="10" r:id="rId5"/>
+    <sheet name="Properties" sheetId="11" r:id="rId6"/>
+    <sheet name="Generation Order" sheetId="9" r:id="rId7"/>
+    <sheet name="Pseudo" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="376">
   <si>
     <t>HexMap - LinkedHashMap&lt;Tuple&lt;Integer&gt;,Hex&gt;</t>
   </si>
@@ -494,30 +493,6 @@
     <t>better way to input biome weights, make it non-compulsory to include biomes, make empty indexes = 0</t>
   </si>
   <si>
-    <t>scrub</t>
-  </si>
-  <si>
-    <t>forest</t>
-  </si>
-  <si>
-    <t>rough</t>
-  </si>
-  <si>
-    <t>desert</t>
-  </si>
-  <si>
-    <t>hills</t>
-  </si>
-  <si>
-    <t>mountains</t>
-  </si>
-  <si>
-    <t>marsh</t>
-  </si>
-  <si>
-    <t>hell</t>
-  </si>
-  <si>
     <t xml:space="preserve">add River generation </t>
   </si>
   <si>
@@ -542,18 +517,6 @@
     <t>these are randomly applied to hexes</t>
   </si>
   <si>
-    <t>TYPE</t>
-  </si>
-  <si>
-    <t>bweight</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>plain</t>
-  </si>
-  <si>
     <t>Hex has: "WorldObjects" - these affect how the hex is treated by programs.</t>
   </si>
   <si>
@@ -1191,6 +1154,12 @@
   </si>
   <si>
     <t>RandomCollection&lt;Biome&gt;&gt; biomes</t>
+  </si>
+  <si>
+    <t>BaseMonster: contains unmodifiable stuff regarding each monster, including its spawn chances.</t>
+  </si>
+  <si>
+    <t>Monster: HAS a basemonster, and whether it’s a lair or nomadic, and other modified stats. THIS HAS THE DESCRIPTOR!!!</t>
   </si>
 </sst>
 </file>
@@ -1662,7 +1631,7 @@
         <v>2</v>
       </c>
       <c r="I16" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="R16" t="s">
         <v>34</v>
@@ -1673,7 +1642,7 @@
         <v>14</v>
       </c>
       <c r="J17" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
@@ -1681,7 +1650,7 @@
         <v>13</v>
       </c>
       <c r="J18" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="Q18" t="s">
         <v>24</v>
@@ -2309,42 +2278,42 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2353,357 +2322,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C3FAB9-666F-4230-B6BA-656A15C724B2}">
-  <dimension ref="A1:J11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E2" t="s">
-        <v>155</v>
-      </c>
-      <c r="F2" t="s">
-        <v>156</v>
-      </c>
-      <c r="G2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H2" t="s">
-        <v>158</v>
-      </c>
-      <c r="I2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B3">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>153</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>156</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>157</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>6</v>
-      </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>158</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>4</v>
-      </c>
-      <c r="H9">
-        <v>8</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>159</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>7</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>160</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>10</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7658268-425E-4714-A5A5-378B4A74F2DC}">
   <dimension ref="B2:W45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2716,152 +2339,152 @@
         <v>1</v>
       </c>
       <c r="V2" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="J3" t="s">
         <v>3</v>
       </c>
       <c r="L3" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="W3" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="J4" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="L4" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="W4" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="E5" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="J5" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="L5" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="E6" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="M6" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="W6" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="N7" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="E8" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="N8" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="E14" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="R14" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="S14" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="S15" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="S16" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="S17" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="R18" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="S18" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="S19" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="E20" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="F20" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">
@@ -2871,67 +2494,67 @@
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="S23" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="U23" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.25">
       <c r="U24" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D26" t="s">
+        <v>186</v>
+      </c>
+      <c r="G26" t="s">
+        <v>196</v>
+      </c>
+      <c r="H26" t="s">
         <v>198</v>
-      </c>
-      <c r="G26" t="s">
-        <v>208</v>
-      </c>
-      <c r="H26" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="D27" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="H27" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="R27" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D28" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="H28" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="D29" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="H29">
         <v>2</v>
@@ -2939,67 +2562,67 @@
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="K31" s="2" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.25">
       <c r="J32" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J33" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J34" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="E42" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="J42" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="E43" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="J43" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="E44" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -3007,7 +2630,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66146DA2-A49A-4A2A-BD60-539D5A363125}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
@@ -3019,129 +2642,532 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="E1" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="N1" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N2" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="O3" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="N4" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="O5" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="N6" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="O7" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="N12" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N13" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="Q13" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N14" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="Q14" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="N15" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="Q15" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="N16" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="Q16" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>244</v>
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E41E48A-940E-466C-A207-70F5A6CF197C}">
+  <dimension ref="B1:W43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>283</v>
+      </c>
+      <c r="N1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>328</v>
+      </c>
+      <c r="R2" t="s">
+        <v>308</v>
+      </c>
+      <c r="S2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>236</v>
+      </c>
+      <c r="P4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Q6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>237</v>
+      </c>
+      <c r="E9" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>323</v>
+      </c>
+      <c r="S9" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>239</v>
+      </c>
+      <c r="E10" t="s">
+        <v>240</v>
+      </c>
+      <c r="I10" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>242</v>
+      </c>
+      <c r="H11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>243</v>
+      </c>
+      <c r="D12" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>275</v>
+      </c>
+      <c r="D13" t="s">
+        <v>274</v>
+      </c>
+      <c r="F13" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>326</v>
+      </c>
+      <c r="E15" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="P17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E19" t="s">
+        <v>314</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>188</v>
+      </c>
+      <c r="S19" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>315</v>
+      </c>
+      <c r="S20" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>319</v>
+      </c>
+      <c r="S21" t="s">
+        <v>320</v>
+      </c>
+      <c r="W21" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>165</v>
+      </c>
+      <c r="W22" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>279</v>
+      </c>
+      <c r="E23" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>280</v>
+      </c>
+      <c r="F24" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>281</v>
+      </c>
+      <c r="F25" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>355</v>
+      </c>
+      <c r="D26" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>285</v>
+      </c>
+      <c r="D28" t="s">
+        <v>286</v>
+      </c>
+      <c r="P28" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>289</v>
+      </c>
+      <c r="D29" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>238</v>
+      </c>
+      <c r="D30" t="s">
+        <v>313</v>
+      </c>
+      <c r="G30" t="s">
+        <v>322</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>287</v>
+      </c>
+      <c r="D31" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>291</v>
+      </c>
+      <c r="D32" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>278</v>
+      </c>
+      <c r="D33" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="34" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>294</v>
+      </c>
+      <c r="D34" t="s">
+        <v>293</v>
+      </c>
+      <c r="G34" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="35" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>299</v>
+      </c>
+      <c r="G35" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="36" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>300</v>
+      </c>
+      <c r="D36" t="s">
+        <v>305</v>
+      </c>
+      <c r="F36" t="s">
+        <v>304</v>
+      </c>
+      <c r="H36" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="37" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>280</v>
+      </c>
+      <c r="E37" t="s">
+        <v>321</v>
+      </c>
+      <c r="I37" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="38" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>281</v>
+      </c>
+      <c r="E38" t="s">
+        <v>321</v>
+      </c>
+      <c r="I38" t="s">
+        <v>312</v>
+      </c>
+      <c r="P38" t="s">
+        <v>330</v>
+      </c>
+      <c r="T38" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="39" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="Q39" t="s">
+        <v>186</v>
+      </c>
+      <c r="U39" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="40" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="Q40" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="41" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="Q41" t="s">
+        <v>331</v>
+      </c>
+      <c r="R41" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="42" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="Q42" t="s">
+        <v>335</v>
+      </c>
+      <c r="R42" t="s">
+        <v>327</v>
+      </c>
+      <c r="T42" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="43" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="Q43" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -3150,401 +3176,133 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E41E48A-940E-466C-A207-70F5A6CF197C}">
-  <dimension ref="B1:W43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533EBB87-5A6A-46A2-9F13-A4D39854AC7D}">
+  <dimension ref="C4:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E1" t="s">
-        <v>295</v>
-      </c>
-      <c r="N1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="O2" t="s">
-        <v>340</v>
-      </c>
-      <c r="R2" t="s">
-        <v>320</v>
-      </c>
-      <c r="S2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="S3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>194</v>
+      </c>
+      <c r="L5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>185</v>
+      </c>
+      <c r="M6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
         <v>248</v>
       </c>
-      <c r="P4" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="Q6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>250</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>249</v>
-      </c>
-      <c r="E9" t="s">
-        <v>294</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>335</v>
-      </c>
-      <c r="S9" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>251</v>
-      </c>
-      <c r="E10" t="s">
-        <v>252</v>
-      </c>
-      <c r="I10" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>254</v>
-      </c>
-      <c r="H11" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>255</v>
-      </c>
-      <c r="D12" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>287</v>
-      </c>
-      <c r="D13" t="s">
-        <v>286</v>
-      </c>
-      <c r="F13" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="F14" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>338</v>
-      </c>
-      <c r="E15" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-      <c r="P17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>200</v>
-      </c>
-      <c r="E19" t="s">
-        <v>326</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>200</v>
-      </c>
-      <c r="S19" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>288</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>327</v>
-      </c>
-      <c r="S20" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>289</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>331</v>
-      </c>
-      <c r="S21" t="s">
-        <v>332</v>
-      </c>
-      <c r="W21" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>290</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>177</v>
-      </c>
-      <c r="W22" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>291</v>
-      </c>
-      <c r="E23" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>292</v>
-      </c>
-      <c r="F24" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>293</v>
-      </c>
-      <c r="F25" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+      <c r="K24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>367</v>
-      </c>
-      <c r="D26" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>297</v>
-      </c>
-      <c r="D28" t="s">
-        <v>298</v>
-      </c>
-      <c r="P28" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>301</v>
-      </c>
-      <c r="D29" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>250</v>
-      </c>
-      <c r="D30" t="s">
-        <v>325</v>
-      </c>
-      <c r="G30" t="s">
-        <v>334</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>299</v>
-      </c>
-      <c r="D31" t="s">
-        <v>300</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>303</v>
-      </c>
-      <c r="D32" t="s">
-        <v>304</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="33" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>290</v>
-      </c>
-      <c r="D33" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="34" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>306</v>
-      </c>
-      <c r="D34" t="s">
-        <v>305</v>
-      </c>
-      <c r="G34" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="35" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>311</v>
-      </c>
-      <c r="G35" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="36" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>312</v>
-      </c>
-      <c r="D36" t="s">
-        <v>317</v>
-      </c>
-      <c r="F36" t="s">
-        <v>316</v>
-      </c>
-      <c r="H36" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="37" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>292</v>
-      </c>
-      <c r="E37" t="s">
-        <v>333</v>
-      </c>
-      <c r="I37" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="38" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>293</v>
-      </c>
-      <c r="E38" t="s">
-        <v>333</v>
-      </c>
-      <c r="I38" t="s">
-        <v>324</v>
-      </c>
-      <c r="P38" t="s">
-        <v>342</v>
-      </c>
-      <c r="T38" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="39" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="Q39" t="s">
-        <v>198</v>
-      </c>
-      <c r="U39" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="40" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="Q40" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="41" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="Q41" t="s">
-        <v>343</v>
-      </c>
-      <c r="R41" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="42" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="Q42" t="s">
-        <v>347</v>
-      </c>
-      <c r="R42" t="s">
-        <v>339</v>
-      </c>
-      <c r="T42" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="43" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="Q43" t="s">
-        <v>311</v>
+        <v>357</v>
+      </c>
+      <c r="K26" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -3553,135 +3311,6 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533EBB87-5A6A-46A2-9F13-A4D39854AC7D}">
-  <dimension ref="C4:N27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>206</v>
-      </c>
-      <c r="L5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>197</v>
-      </c>
-      <c r="M6" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>260</v>
-      </c>
-      <c r="L12" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="L13" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="L14" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="M15" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="N16" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>370</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD20796D-B0DE-4732-BD5F-0F3C623F8AF6}">
   <dimension ref="B1:I17"/>
   <sheetViews>
@@ -3693,91 +3322,91 @@
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="H5" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="H12" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="I12" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds town finder to improve road pathing.
</commit_message>
<xml_diff>
--- a/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
+++ b/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keeley\git\HexCrawlRepo\HexCrawlGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBE3E1C-058A-4DDA-B851-5E2F5467F578}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D49182-A93E-4B4D-AF19-9F0266ED7A51}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="4" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="6" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -2729,7 +2729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E41E48A-940E-466C-A207-70F5A6CF197C}">
   <dimension ref="B1:W43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
@@ -3285,8 +3285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD20796D-B0DE-4732-BD5F-0F3C623F8AF6}">
   <dimension ref="B1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U13" sqref="U13:V13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
finds bug in roadfinding algorithm,
no longer need town finder to do additional connections
</commit_message>
<xml_diff>
--- a/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
+++ b/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keeley\git\HexCrawlRepo\HexCrawlGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D49182-A93E-4B4D-AF19-9F0266ED7A51}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5458857-D156-4D14-8939-13A7607D0C90}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="6" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="414">
   <si>
     <t>HexMap - LinkedHashMap&lt;Tuple&lt;Integer&gt;,Hex&gt;</t>
   </si>
@@ -1158,6 +1158,123 @@
   <si>
     <t>default is all:1</t>
   </si>
+  <si>
+    <t>Road cleaner</t>
+  </si>
+  <si>
+    <t>Iterate through roadnodes, get connection size.</t>
+  </si>
+  <si>
+    <t>----------------</t>
+  </si>
+  <si>
+    <t>Set&lt;RoadNode&gt; roadnodes</t>
+  </si>
+  <si>
+    <t>Set&lt;Connection&gt; roadconnections</t>
+  </si>
+  <si>
+    <t>clean(set node, set connection</t>
+  </si>
+  <si>
+    <t>For each roadnetwork</t>
+  </si>
+  <si>
+    <t>from roadnetwork</t>
+  </si>
+  <si>
+    <t>remove nodes, remove connections</t>
+  </si>
+  <si>
+    <t>Add all roadnodes w/ connection size &gt; 2 to Set intersectionNodes</t>
+  </si>
+  <si>
+    <t>recursiveTravel(node, visitedN, visitedC)</t>
+  </si>
+  <si>
+    <t>---------------</t>
+  </si>
+  <si>
+    <t>set visitedC = new</t>
+  </si>
+  <si>
+    <t>set visitedN = new</t>
+  </si>
+  <si>
+    <t>Iterate through each node in set intersectionNode</t>
+  </si>
+  <si>
+    <t>for each connection from node not in visitedC</t>
+  </si>
+  <si>
+    <t>visitedN+=node</t>
+  </si>
+  <si>
+    <t>nodeO = connection.other</t>
+  </si>
+  <si>
+    <t>if nodeO is in set visitedN</t>
+  </si>
+  <si>
+    <t>if nodeO is not in set R</t>
+  </si>
+  <si>
+    <t>if node ! Contain town</t>
+  </si>
+  <si>
+    <t>visitedC +=connection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">else </t>
+  </si>
+  <si>
+    <t>vistedN+=nodeO</t>
+  </si>
+  <si>
+    <t>delete = recursiveTravel(node, visitedN, visitedC)</t>
+  </si>
+  <si>
+    <t>return false;</t>
+  </si>
+  <si>
+    <t>return true;</t>
+  </si>
+  <si>
+    <t>if (delete) &amp;&amp; this node ! In set R</t>
+  </si>
+  <si>
+    <t>delete connection from and to this node, delete this node</t>
+  </si>
+  <si>
+    <t>check nodeO still valid in set R</t>
+  </si>
+  <si>
+    <t>PARTLY DONE</t>
+  </si>
+  <si>
+    <t>Add complex string printouts</t>
+  </si>
+  <si>
+    <t>Add settings file to modify all inputs</t>
+  </si>
+  <si>
+    <t>Add basic string printouts for each hex</t>
+  </si>
+  <si>
+    <t>Add intuitive coordinate system</t>
+  </si>
+  <si>
+    <t>Add "stats" handling/rolls</t>
+  </si>
+  <si>
+    <t>Add "centre-start" generation option</t>
+  </si>
+  <si>
+    <t>Add biome regoins</t>
+  </si>
+  <si>
+    <t>Add minimum size biome setting</t>
+  </si>
 </sst>
 </file>
 
@@ -2573,10 +2690,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66146DA2-A49A-4A2A-BD60-539D5A363125}">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="N11" sqref="H10:N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2609,8 +2726,11 @@
       <c r="A4" t="s">
         <v>215</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>370</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>369</v>
       </c>
       <c r="N4" t="s">
         <v>239</v>
@@ -2620,7 +2740,7 @@
       <c r="A5" t="s">
         <v>220</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>369</v>
       </c>
       <c r="O5" t="s">
@@ -2631,6 +2751,9 @@
       <c r="A6" t="s">
         <v>258</v>
       </c>
+      <c r="G6" s="4" t="s">
+        <v>405</v>
+      </c>
       <c r="N6" t="s">
         <v>240</v>
       </c>
@@ -2639,6 +2762,9 @@
       <c r="A7" t="s">
         <v>221</v>
       </c>
+      <c r="G7" s="5" t="s">
+        <v>369</v>
+      </c>
       <c r="O7" t="s">
         <v>242</v>
       </c>
@@ -2647,8 +2773,11 @@
       <c r="A8" t="s">
         <v>257</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>371</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -2665,7 +2794,7 @@
       <c r="A11" t="s">
         <v>256</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>371</v>
       </c>
     </row>
@@ -2695,7 +2824,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>217</v>
+        <v>411</v>
       </c>
       <c r="N15" t="s">
         <v>252</v>
@@ -2706,7 +2835,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>218</v>
+        <v>410</v>
       </c>
       <c r="N16" t="s">
         <v>253</v>
@@ -2715,9 +2844,49 @@
         <v>254</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -3283,35 +3452,35 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD20796D-B0DE-4732-BD5F-0F3C623F8AF6}">
-  <dimension ref="B1:I17"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>324</v>
       </c>
@@ -3319,32 +3488,32 @@
         <v>339</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>329</v>
       </c>
@@ -3355,29 +3524,187 @@
         <v>340</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>331</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>375</v>
+      </c>
+      <c r="G23" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Formatting and preparing to start work on view printouts
</commit_message>
<xml_diff>
--- a/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
+++ b/HexCrawlGenerator/HexCrawlBrainstorming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keeley\git\HexCrawlRepo\HexCrawlGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5458857-D156-4D14-8939-13A7607D0C90}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AFB8DA-C7C3-46BD-A547-2B0FA65AE24F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="6" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="8" xr2:uid="{87C68EA5-05F6-40AA-A0F5-E044F78FA25B}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Generation Order" sheetId="9" r:id="rId6"/>
     <sheet name="Pseudo" sheetId="12" r:id="rId7"/>
     <sheet name="Fixed neighbour error" sheetId="13" r:id="rId8"/>
+    <sheet name="View" sheetId="14" r:id="rId9"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="448">
   <si>
     <t>HexMap - LinkedHashMap&lt;Tuple&lt;Integer&gt;,Hex&gt;</t>
   </si>
@@ -1275,13 +1276,156 @@
   <si>
     <t>Add minimum size biome setting</t>
   </si>
+  <si>
+    <t>Rename this to a biome layer</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">spawnchances can be on </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>either</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> biomes or biome-layers.</t>
+    </r>
+  </si>
+  <si>
+    <t>Module Based</t>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>Lairs / Dungeons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visiting / Nomadic </t>
+  </si>
+  <si>
+    <t>Towns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIGNPOST: Towns along each road with distance + time taken </t>
+  </si>
+  <si>
+    <t>Monsters, name and number</t>
+  </si>
+  <si>
+    <t>Each "neighbouring" unique region to current region</t>
+  </si>
+  <si>
+    <t>This Hex</t>
+  </si>
+  <si>
+    <t>Neighbouring unique biomes</t>
+  </si>
+  <si>
+    <t>name, direction</t>
+  </si>
+  <si>
+    <t>Distant tall regions within sight (40mi)</t>
+  </si>
+  <si>
+    <t>Navigation Priorities</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>name, direction, distance</t>
+  </si>
+  <si>
+    <t>distance (if applicable)</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>This River</t>
+  </si>
+  <si>
+    <t>Closest Unique Region up/downstream from here</t>
+  </si>
+  <si>
+    <t>Source + Destination Region &amp; Hex Coordinate</t>
+  </si>
+  <si>
+    <t>name, direction, coordinate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">region name, river coordinate </t>
+  </si>
+  <si>
+    <t>region name, river coordinate, distance</t>
+  </si>
+  <si>
+    <t>name, direction (center-center)</t>
+  </si>
+  <si>
+    <t>River Priorities</t>
+  </si>
+  <si>
+    <t>region name</t>
+  </si>
+  <si>
+    <t>coordinate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waypoints </t>
+  </si>
+  <si>
+    <t>name, description</t>
+  </si>
+  <si>
+    <t>Each road direction:</t>
+  </si>
+  <si>
+    <t>towns, distance, travel-time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1336,13 +1480,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2898,8 +3043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E41E48A-940E-466C-A207-70F5A6CF197C}">
   <dimension ref="B1:W43"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3204,7 +3349,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>265</v>
       </c>
@@ -3212,7 +3357,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="34" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>281</v>
       </c>
@@ -3223,7 +3368,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="35" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>285</v>
       </c>
@@ -3231,7 +3376,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="36" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>286</v>
       </c>
@@ -3245,7 +3390,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="37" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>267</v>
       </c>
@@ -3256,7 +3401,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="38" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>268</v>
       </c>
@@ -3273,7 +3418,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="39" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="Q39" t="s">
         <v>173</v>
       </c>
@@ -3281,12 +3426,15 @@
         <v>320</v>
       </c>
     </row>
-    <row r="40" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="Q40" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="41" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>414</v>
+      </c>
       <c r="Q41" t="s">
         <v>317</v>
       </c>
@@ -3294,7 +3442,10 @@
         <v>318</v>
       </c>
     </row>
-    <row r="42" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>415</v>
+      </c>
       <c r="Q42" t="s">
         <v>321</v>
       </c>
@@ -3305,13 +3456,14 @@
         <v>322</v>
       </c>
     </row>
-    <row r="43" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="Q43" t="s">
         <v>285</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3454,7 +3606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD20796D-B0DE-4732-BD5F-0F3C623F8AF6}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -67995,4 +68147,220 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669B5755-9301-4059-BC46-2020EE4ADC49}">
+  <dimension ref="A2:H40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>428</v>
+      </c>
+      <c r="E4" t="s">
+        <v>417</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
+        <v>429</v>
+      </c>
+      <c r="F5" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>430</v>
+      </c>
+      <c r="G6" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>432</v>
+      </c>
+      <c r="H7" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>433</v>
+      </c>
+      <c r="F8" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>441</v>
+      </c>
+      <c r="E16" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>100</v>
+      </c>
+      <c r="B17" t="s">
+        <v>442</v>
+      </c>
+      <c r="F17" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>443</v>
+      </c>
+      <c r="G18" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>432</v>
+      </c>
+      <c r="H19" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>433</v>
+      </c>
+      <c r="F20" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>420</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>